<commit_message>
matrix and few details
</commit_message>
<xml_diff>
--- a/matrice d'implication GL.xlsx
+++ b/matrice d'implication GL.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCBD4AA-BCBB-44BA-810D-F699048E4755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C1B9C9-C3AB-4900-9ADB-8FB63EEC39E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,36 +526,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -584,6 +554,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -890,42 +890,42 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="2:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="22" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="28" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="38"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="16" t="s">
@@ -937,7 +937,7 @@
       <c r="D6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -948,10 +948,10 @@
       <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="24">
         <v>0.5</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="28">
         <v>0.5</v>
       </c>
     </row>
@@ -963,10 +963,10 @@
       <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="24">
         <v>0.5</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="27">
         <v>0.5</v>
       </c>
     </row>
@@ -978,10 +978,10 @@
       <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="24">
         <v>0.5</v>
       </c>
-      <c r="E9" s="37">
+      <c r="E9" s="27">
         <v>0.5</v>
       </c>
     </row>
@@ -993,11 +993,11 @@
       <c r="C10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="34">
-        <v>0.1</v>
-      </c>
-      <c r="E10" s="37">
-        <v>0.9</v>
+      <c r="D10" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="E10" s="27">
+        <v>0.7</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
@@ -1008,11 +1008,11 @@
       <c r="C11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="34">
-        <v>0.9</v>
-      </c>
-      <c r="E11" s="37">
-        <v>0.1</v>
+      <c r="D11" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="E11" s="27">
+        <v>0.3</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
@@ -1023,11 +1023,11 @@
       <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="34">
-        <v>0.9</v>
-      </c>
-      <c r="E12" s="37">
-        <v>0.1</v>
+      <c r="D12" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="E12" s="27">
+        <v>0.3</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
@@ -1038,11 +1038,11 @@
       <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="34">
-        <v>0.9</v>
-      </c>
-      <c r="E13" s="37">
-        <v>0.1</v>
+      <c r="D13" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="E13" s="27">
+        <v>0.3</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
@@ -1053,10 +1053,10 @@
       <c r="C14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="34">
-        <v>1</v>
-      </c>
-      <c r="E14" s="37">
+      <c r="D14" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="E14" s="27">
         <v>0.1</v>
       </c>
     </row>
@@ -1068,10 +1068,10 @@
       <c r="C15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="24">
         <v>0.5</v>
       </c>
-      <c r="E15" s="37">
+      <c r="E15" s="27">
         <v>0.5</v>
       </c>
     </row>
@@ -1081,8 +1081,8 @@
         <v>10</v>
       </c>
       <c r="C16" s="6"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="35"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="4">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="35"/>
+      <c r="E17" s="25"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="4">
@@ -1100,7 +1100,7 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="35"/>
+      <c r="E18" s="25"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="4">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="35"/>
+      <c r="E19" s="25"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="4">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="35"/>
+      <c r="E20" s="25"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="4">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="35"/>
+      <c r="E21" s="25"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="4">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="35"/>
+      <c r="E22" s="25"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="4">
@@ -1145,7 +1145,7 @@
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="35"/>
+      <c r="E23" s="25"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="4">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="35"/>
+      <c r="E24" s="25"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="4">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="35"/>
+      <c r="E25" s="25"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="4">
@@ -1172,7 +1172,7 @@
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="35"/>
+      <c r="E26" s="25"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="4">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="35"/>
+      <c r="E27" s="25"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="4">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="35"/>
+      <c r="E28" s="25"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="4">
@@ -1199,7 +1199,7 @@
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="35"/>
+      <c r="E29" s="25"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="4">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="35"/>
+      <c r="E30" s="25"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="4">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="8"/>
-      <c r="E31" s="35"/>
+      <c r="E31" s="25"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="4">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="8"/>
-      <c r="E32" s="35"/>
+      <c r="E32" s="25"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="4">
@@ -1235,7 +1235,7 @@
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="8"/>
-      <c r="E33" s="35"/>
+      <c r="E33" s="25"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="4">
@@ -1244,13 +1244,13 @@
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="8"/>
-      <c r="E34" s="35"/>
+      <c r="E34" s="25"/>
     </row>
     <row r="35" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="5"/>
       <c r="C35" s="7"/>
       <c r="D35" s="9"/>
-      <c r="E35" s="36"/>
+      <c r="E35" s="26"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="15" t="s">

</xml_diff>